<commit_message>
WIP belongstoMany for Words
</commit_message>
<xml_diff>
--- a/database/vox_data.xlsx
+++ b/database/vox_data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28315"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Xavier/Documents/CPNV/Modules/2018-2019/T2/PRW2/Projets/Voxerver/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Senistan.JEGARAJASIN\Desktop\Github Projects\Voxerver\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-4540" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="-4545" yWindow="-21135" windowWidth="38400" windowHeight="21135" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -653,7 +653,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -744,6 +744,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1071,24 +1074,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H111"/>
+  <dimension ref="A1:R111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H118" sqref="H118"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K79" sqref="K79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="61" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="58.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="56.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>197</v>
       </c>
@@ -1097,7 +1102,7 @@
         <v>INSERT INTO languages (languageName) VALUES ('Français');</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>198</v>
       </c>
@@ -1106,10 +1111,10 @@
         <v>INSERT INTO languages (languageName) VALUES ('Anglais');</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1118,7 +1123,7 @@
         <v>INSERT INTO themes (title) VALUES ('Banking');</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1127,7 +1132,7 @@
         <v>INSERT INTO themes (title) VALUES ('Furniture');</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1136,7 +1141,7 @@
         <v>INSERT INTO themes (title) VALUES ('Colors');</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1145,7 +1150,7 @@
         <v>INSERT INTO themes (title) VALUES ('Family Members');</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1175,8 +1180,19 @@
         <f>"INSERT INTO words(value,language_id,semantic_id) VALUES ('"&amp;D9&amp;"',2," &amp; ROW()-8 &amp; ");"</f>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the bank',2,1);</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K9" t="str">
+        <f>"INSERT INTO contents(theme_id,word_id) VALUES('"&amp;A9&amp;"','"&amp;F9&amp;"');"</f>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','1');</v>
+      </c>
+      <c r="M9" t="str">
+        <f>"INSERT INTO contents(theme_id,word_id) VALUES('"&amp;A9&amp;"','"&amp;R9&amp;"');"</f>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','104');</v>
+      </c>
+      <c r="R9">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1206,8 +1222,19 @@
         <f t="shared" ref="H10:H73" si="6">"INSERT INTO words(value,language_id,semantic_id) VALUES ('"&amp;D10&amp;"',2," &amp; ROW()-8 &amp; ");"</f>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('cash',2,2);</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K10" t="str">
+        <f t="shared" ref="K10:K73" si="7">"INSERT INTO contents(theme_id,word_id) VALUES('"&amp;A10&amp;"','"&amp;F10&amp;"');"</f>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','2');</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" ref="M10:M73" si="8">"INSERT INTO contents(theme_id,word_id) VALUES('"&amp;A10&amp;"','"&amp;R10&amp;"');"</f>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','105');</v>
+      </c>
+      <c r="R10">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1237,8 +1264,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('payment',2,3);</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K11" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','3');</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','106');</v>
+      </c>
+      <c r="R11">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1268,8 +1306,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('checkbook',2,4);</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K12" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','4');</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','107');</v>
+      </c>
+      <c r="R12">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1299,8 +1348,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('to deposit money',2,5);</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K13" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','5');</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','108');</v>
+      </c>
+      <c r="R13">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1330,8 +1390,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('to borrow money',2,6);</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K14" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','6');</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','109');</v>
+      </c>
+      <c r="R14">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1361,8 +1432,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('financial services',2,7);</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K15" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','7');</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','110');</v>
+      </c>
+      <c r="R15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1392,8 +1474,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('commission',2,8);</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K16" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','8');</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','111');</v>
+      </c>
+      <c r="R16">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1423,8 +1516,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('an investment',2,9);</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K17" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','9');</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','112');</v>
+      </c>
+      <c r="R17">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1454,8 +1558,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('transfer',2,10);</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K18" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','10');</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','113');</v>
+      </c>
+      <c r="R18">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1485,8 +1600,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('money management',2,11);</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K19" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','11');</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','114');</v>
+      </c>
+      <c r="R19">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1516,8 +1642,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a transaction',2,12);</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K20" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','12');</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','115');</v>
+      </c>
+      <c r="R20">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1547,8 +1684,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('ATM machine',2,13);</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K21" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','13');</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','116');</v>
+      </c>
+      <c r="R21">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1578,8 +1726,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('to wait in line',2,14);</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K22" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','14');</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','117');</v>
+      </c>
+      <c r="R22">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1609,8 +1768,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('banking/ATM card',2,15);</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K23" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','15');</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','118');</v>
+      </c>
+      <c r="R23">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1640,8 +1810,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('to save money',2,16);</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K24" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','16');</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','119');</v>
+      </c>
+      <c r="R24">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1671,8 +1852,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('sum/total amount',2,17);</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K25" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','17');</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','120');</v>
+      </c>
+      <c r="R25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1702,8 +1894,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('checking account',2,18);</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K26" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','18');</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','121');</v>
+      </c>
+      <c r="R26">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1733,8 +1936,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('money',2,19);</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K27" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','19');</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','122');</v>
+      </c>
+      <c r="R27">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1764,8 +1978,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('funds',2,20);</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K28" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','20');</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','123');</v>
+      </c>
+      <c r="R28">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1795,8 +2020,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('check',2,21);</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K29" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','21');</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','124');</v>
+      </c>
+      <c r="R29">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1826,8 +2062,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('deposit',2,22);</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K30" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','22');</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','125');</v>
+      </c>
+      <c r="R30">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1857,8 +2104,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('credit',2,23);</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K31" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','23');</v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','126');</v>
+      </c>
+      <c r="R31">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1888,8 +2146,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('financial markets',2,24);</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K32" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','24');</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','127');</v>
+      </c>
+      <c r="R32">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1919,8 +2188,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('clientele',2,25);</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K33" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','25');</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','128');</v>
+      </c>
+      <c r="R33">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1950,8 +2230,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('fees',2,26);</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K34" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','26');</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','129');</v>
+      </c>
+      <c r="R34">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1981,8 +2272,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('financial institution',2,27);</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K35" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','27');</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','130');</v>
+      </c>
+      <c r="R35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -2012,8 +2314,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('interest rate',2,28);</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K36" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','28');</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','131');</v>
+      </c>
+      <c r="R36">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2043,8 +2356,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('currency',2,29);</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K37" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','29');</v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','132');</v>
+      </c>
+      <c r="R37">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -2074,8 +2398,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('balance',2,30);</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K38" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','30');</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','133');</v>
+      </c>
+      <c r="R38">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2105,8 +2440,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('to take a number',2,31);</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K39" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','31');</v>
+      </c>
+      <c r="M39" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','134');</v>
+      </c>
+      <c r="R39">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1</v>
       </c>
@@ -2136,8 +2482,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('credit card',2,32);</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K40" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','32');</v>
+      </c>
+      <c r="M40" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','135');</v>
+      </c>
+      <c r="R40">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -2167,8 +2524,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a loan',2,33);</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K41" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','33');</v>
+      </c>
+      <c r="M41" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','136');</v>
+      </c>
+      <c r="R41">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -2198,8 +2566,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('to take out money',2,34);</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K42" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','34');</v>
+      </c>
+      <c r="M42" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','137');</v>
+      </c>
+      <c r="R42">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -2229,8 +2608,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('savings account',2,35);</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K43" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','35');</v>
+      </c>
+      <c r="M43" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','138');</v>
+      </c>
+      <c r="R43">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -2260,8 +2650,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('ATM machine',2,36);</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K44" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','36');</v>
+      </c>
+      <c r="M44" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','139');</v>
+      </c>
+      <c r="R44">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -2291,8 +2692,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('receipt',2,37);</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K45" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','37');</v>
+      </c>
+      <c r="M45" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('1','140');</v>
+      </c>
+      <c r="R45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2</v>
       </c>
@@ -2322,8 +2734,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a table',2,38);</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K46" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','38');</v>
+      </c>
+      <c r="M46" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','141');</v>
+      </c>
+      <c r="R46">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <f>A46</f>
         <v>2</v>
@@ -2354,10 +2777,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a chair',2,39);</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K47" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','39');</v>
+      </c>
+      <c r="M47" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','142');</v>
+      </c>
+      <c r="R47">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" ref="A48:A111" si="7">A47</f>
+        <f t="shared" ref="A48:A111" si="9">A47</f>
         <v>2</v>
       </c>
       <c r="B48" t="s">
@@ -2386,10 +2820,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a bookcase',2,40);</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K48" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','40');</v>
+      </c>
+      <c r="M48" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','143');</v>
+      </c>
+      <c r="R48">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B49" t="s">
@@ -2418,10 +2863,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a coffee table',2,41);</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K49" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','41');</v>
+      </c>
+      <c r="M49" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','144');</v>
+      </c>
+      <c r="R49">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B50" t="s">
@@ -2450,10 +2906,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a fireplace',2,42);</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K50" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','42');</v>
+      </c>
+      <c r="M50" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','145');</v>
+      </c>
+      <c r="R50">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B51" t="s">
@@ -2482,10 +2949,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a bedside table',2,43);</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K51" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','43');</v>
+      </c>
+      <c r="M51" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','146');</v>
+      </c>
+      <c r="R51">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B52" t="s">
@@ -2514,10 +2992,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a shelf',2,44);</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K52" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','44');</v>
+      </c>
+      <c r="M52" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','147');</v>
+      </c>
+      <c r="R52">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B53" t="s">
@@ -2546,10 +3035,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a wardrobe',2,45);</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K53" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','45');</v>
+      </c>
+      <c r="M53" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','148');</v>
+      </c>
+      <c r="R53">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B54" t="s">
@@ -2578,10 +3078,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a dresser',2,46);</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K54" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','46');</v>
+      </c>
+      <c r="M54" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','149');</v>
+      </c>
+      <c r="R54">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B55" t="s">
@@ -2610,10 +3121,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a carpet',2,47);</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K55" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','47');</v>
+      </c>
+      <c r="M55" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','150');</v>
+      </c>
+      <c r="R55">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B56" t="s">
@@ -2642,10 +3164,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a seat',2,48);</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K56" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','48');</v>
+      </c>
+      <c r="M56" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','151');</v>
+      </c>
+      <c r="R56">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B57" t="s">
@@ -2674,10 +3207,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a stool',2,49);</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K57" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','49');</v>
+      </c>
+      <c r="M57" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','152');</v>
+      </c>
+      <c r="R57">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B58" t="s">
@@ -2706,10 +3250,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a cupboard',2,50);</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K58" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','50');</v>
+      </c>
+      <c r="M58" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','153');</v>
+      </c>
+      <c r="R58">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B59" t="s">
@@ -2738,10 +3293,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a drawer',2,51);</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K59" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','51');</v>
+      </c>
+      <c r="M59" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','154');</v>
+      </c>
+      <c r="R59">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B60" t="s">
@@ -2770,10 +3336,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a armchair',2,52);</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K60" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','52');</v>
+      </c>
+      <c r="M60" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','155');</v>
+      </c>
+      <c r="R60">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B61" t="s">
@@ -2802,10 +3379,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a bed',2,53);</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K61" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','53');</v>
+      </c>
+      <c r="M61" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','156');</v>
+      </c>
+      <c r="R61">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B62" t="s">
@@ -2834,10 +3422,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a desk',2,54);</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K62" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','54');</v>
+      </c>
+      <c r="M62" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','157');</v>
+      </c>
+      <c r="R62">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B63" t="s">
@@ -2866,10 +3465,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a mrror',2,55);</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K63" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','55');</v>
+      </c>
+      <c r="M63" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','158');</v>
+      </c>
+      <c r="R63">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B64" t="s">
@@ -2898,10 +3508,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a piece of furniture',2,56);</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K64" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','56');</v>
+      </c>
+      <c r="M64" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','159');</v>
+      </c>
+      <c r="R64">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B65" t="s">
@@ -2930,8 +3551,19 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('a pillow',2,57);</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K65" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','57');</v>
+      </c>
+      <c r="M65" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('2','160');</v>
+      </c>
+      <c r="R65">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>3</v>
       </c>
@@ -2961,10 +3593,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('white',2,58);</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K66" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','58');</v>
+      </c>
+      <c r="M66" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','161');</v>
+      </c>
+      <c r="R66">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B67" t="s">
@@ -2993,10 +3636,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('light blue',2,59);</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K67" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','59');</v>
+      </c>
+      <c r="M67" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','162');</v>
+      </c>
+      <c r="R67">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B68" t="s">
@@ -3025,10 +3679,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('muli-colored',2,60);</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K68" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','60');</v>
+      </c>
+      <c r="M68" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','163');</v>
+      </c>
+      <c r="R68">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B69" t="s">
@@ -3057,10 +3722,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('grey',2,61);</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K69" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','61');</v>
+      </c>
+      <c r="M69" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','164');</v>
+      </c>
+      <c r="R69">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B70" t="s">
@@ -3089,10 +3765,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('green',2,62);</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K70" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','62');</v>
+      </c>
+      <c r="M70" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','165');</v>
+      </c>
+      <c r="R70">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B71" t="s">
@@ -3121,10 +3808,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('black',2,63);</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K71" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','63');</v>
+      </c>
+      <c r="M71" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','166');</v>
+      </c>
+      <c r="R71">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B72" t="s">
@@ -3153,10 +3851,21 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('silver',2,64);</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K72" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','64');</v>
+      </c>
+      <c r="M72" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','167');</v>
+      </c>
+      <c r="R72">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B73" t="s">
@@ -3185,328 +3894,449 @@
         <f t="shared" si="6"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('yellow',2,65);</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K73" t="str">
+        <f t="shared" si="7"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','65');</v>
+      </c>
+      <c r="M73" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','168');</v>
+      </c>
+      <c r="R73">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B74" t="s">
         <v>125</v>
       </c>
       <c r="C74">
-        <f t="shared" ref="C74:C111" si="8">(ROW()-9)*2+1</f>
+        <f t="shared" ref="C74:C111" si="10">(ROW()-9)*2+1</f>
         <v>131</v>
       </c>
       <c r="D74" t="s">
         <v>125</v>
       </c>
       <c r="E74">
-        <f t="shared" ref="E74:E111" si="9">(ROW()-9)*2+2</f>
+        <f t="shared" ref="E74:E111" si="11">(ROW()-9)*2+2</f>
         <v>132</v>
       </c>
       <c r="F74">
-        <f t="shared" ref="F74:F111" si="10">(ROW()-8)</f>
+        <f t="shared" ref="F74:F111" si="12">(ROW()-8)</f>
         <v>66</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" ref="G74:G111" si="11">"INSERT INTO words(value,language_id,semantic_id) VALUES ('"&amp;B74&amp;"',1," &amp; ROW()-8 &amp; ");"</f>
+        <f t="shared" ref="G74:G111" si="13">"INSERT INTO words(value,language_id,semantic_id) VALUES ('"&amp;B74&amp;"',1," &amp; ROW()-8 &amp; ");"</f>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('orange',1,66);</v>
       </c>
       <c r="H74" t="str">
-        <f t="shared" ref="H74:H111" si="12">"INSERT INTO words(value,language_id,semantic_id) VALUES ('"&amp;D74&amp;"',2," &amp; ROW()-8 &amp; ");"</f>
+        <f t="shared" ref="H74:H111" si="14">"INSERT INTO words(value,language_id,semantic_id) VALUES ('"&amp;D74&amp;"',2," &amp; ROW()-8 &amp; ");"</f>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('orange',2,66);</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K74" t="str">
+        <f t="shared" ref="K74:K111" si="15">"INSERT INTO contents(theme_id,word_id) VALUES('"&amp;A74&amp;"','"&amp;F74&amp;"');"</f>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','66');</v>
+      </c>
+      <c r="M74" t="str">
+        <f t="shared" ref="M74:M111" si="16">"INSERT INTO contents(theme_id,word_id) VALUES('"&amp;A74&amp;"','"&amp;R74&amp;"');"</f>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','169');</v>
+      </c>
+      <c r="R74">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B75" t="s">
         <v>126</v>
       </c>
       <c r="C75">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>133</v>
       </c>
       <c r="D75" t="s">
         <v>127</v>
       </c>
       <c r="E75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>134</v>
       </c>
       <c r="F75">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>67</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('bleu',1,67);</v>
       </c>
       <c r="H75" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('blue',2,67);</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K75" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','67');</v>
+      </c>
+      <c r="M75" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','170');</v>
+      </c>
+      <c r="R75">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B76" t="s">
         <v>128</v>
       </c>
       <c r="C76">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>135</v>
       </c>
       <c r="D76" t="s">
         <v>129</v>
       </c>
       <c r="E76">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>136</v>
       </c>
       <c r="F76">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>68</v>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('bleu foncé',1,68);</v>
       </c>
       <c r="H76" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('dark blue',2,68);</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K76" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','68');</v>
+      </c>
+      <c r="M76" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','171');</v>
+      </c>
+      <c r="R76">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B77" t="s">
         <v>130</v>
       </c>
       <c r="C77">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>137</v>
       </c>
       <c r="D77" t="s">
         <v>131</v>
       </c>
       <c r="E77">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>138</v>
       </c>
       <c r="F77">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>69</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('rose',1,69);</v>
       </c>
       <c r="H77" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('pink',2,69);</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K77" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','69');</v>
+      </c>
+      <c r="M77" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','172');</v>
+      </c>
+      <c r="R77">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B78" t="s">
         <v>132</v>
       </c>
       <c r="C78">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>139</v>
       </c>
       <c r="D78" t="s">
         <v>133</v>
       </c>
       <c r="E78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>140</v>
       </c>
       <c r="F78">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>70</v>
       </c>
       <c r="G78" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('rouge',1,70);</v>
       </c>
       <c r="H78" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('red',2,70);</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K78" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','70');</v>
+      </c>
+      <c r="M78" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','173');</v>
+      </c>
+      <c r="R78">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B79" t="s">
         <v>134</v>
       </c>
       <c r="C79">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>141</v>
       </c>
       <c r="D79" t="s">
         <v>135</v>
       </c>
       <c r="E79">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>142</v>
       </c>
       <c r="F79">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>71</v>
       </c>
       <c r="G79" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('marron',1,71);</v>
       </c>
       <c r="H79" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('brown',2,71);</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K79" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','71');</v>
+      </c>
+      <c r="M79" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','174');</v>
+      </c>
+      <c r="R79">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B80" t="s">
         <v>136</v>
       </c>
       <c r="C80">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>143</v>
       </c>
       <c r="D80" t="s">
         <v>137</v>
       </c>
       <c r="E80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>144</v>
       </c>
       <c r="F80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>72</v>
       </c>
       <c r="G80" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('violet',1,72);</v>
       </c>
       <c r="H80" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('purple',2,72);</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K80" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','72');</v>
+      </c>
+      <c r="M80" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','175');</v>
+      </c>
+      <c r="R80">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B81" t="s">
         <v>138</v>
       </c>
       <c r="C81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>145</v>
       </c>
       <c r="D81" t="s">
         <v>138</v>
       </c>
       <c r="E81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>146</v>
       </c>
       <c r="F81">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>73</v>
       </c>
       <c r="G81" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('beige',1,73);</v>
       </c>
       <c r="H81" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('beige',2,73);</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K81" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','73');</v>
+      </c>
+      <c r="M81" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','176');</v>
+      </c>
+      <c r="R81">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B82" t="s">
         <v>139</v>
       </c>
       <c r="C82">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>147</v>
       </c>
       <c r="D82" t="s">
         <v>139</v>
       </c>
       <c r="E82">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>148</v>
       </c>
       <c r="F82">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>74</v>
       </c>
       <c r="G82" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('turquoise',1,74);</v>
       </c>
       <c r="H82" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('turquoise',2,74);</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K82" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','74');</v>
+      </c>
+      <c r="M82" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','177');</v>
+      </c>
+      <c r="R82">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B83" t="s">
         <v>140</v>
       </c>
       <c r="C83">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>149</v>
       </c>
       <c r="D83" t="s">
         <v>141</v>
       </c>
       <c r="E83">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>150</v>
       </c>
       <c r="F83">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>75</v>
       </c>
       <c r="G83" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('doré',1,75);</v>
       </c>
       <c r="H83" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('golden',2,75);</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K83" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','75');</v>
+      </c>
+      <c r="M83" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('3','178');</v>
+      </c>
+      <c r="R83">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>4</v>
       </c>
@@ -3514,891 +4344,1199 @@
         <v>142</v>
       </c>
       <c r="C84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>151</v>
       </c>
       <c r="D84" t="s">
         <v>143</v>
       </c>
       <c r="E84">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>152</v>
       </c>
       <c r="F84">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>76</v>
       </c>
       <c r="G84" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('le père',1,76);</v>
       </c>
       <c r="H84" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the father',2,76);</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K84" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','76');</v>
+      </c>
+      <c r="M84" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','179');</v>
+      </c>
+      <c r="R84">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B85" t="s">
         <v>144</v>
       </c>
       <c r="C85">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>153</v>
       </c>
       <c r="D85" t="s">
         <v>145</v>
       </c>
       <c r="E85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>154</v>
       </c>
       <c r="F85">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>77</v>
       </c>
       <c r="G85" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('les parents',1,77);</v>
       </c>
       <c r="H85" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the parents',2,77);</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K85" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','77');</v>
+      </c>
+      <c r="M85" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','180');</v>
+      </c>
+      <c r="R85">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B86" t="s">
         <v>146</v>
       </c>
       <c r="C86">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>155</v>
       </c>
       <c r="D86" t="s">
         <v>147</v>
       </c>
       <c r="E86">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>156</v>
       </c>
       <c r="F86">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>78</v>
       </c>
       <c r="G86" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('la sœur',1,78);</v>
       </c>
       <c r="H86" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the sister',2,78);</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K86" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','78');</v>
+      </c>
+      <c r="M86" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','181');</v>
+      </c>
+      <c r="R86">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B87" t="s">
         <v>148</v>
       </c>
       <c r="C87">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>157</v>
       </c>
       <c r="D87" t="s">
         <v>149</v>
       </c>
       <c r="E87">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>158</v>
       </c>
       <c r="F87">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>79</v>
       </c>
       <c r="G87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('la fille',1,79);</v>
       </c>
       <c r="H87" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the daughter',2,79);</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K87" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','79');</v>
+      </c>
+      <c r="M87" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','182');</v>
+      </c>
+      <c r="R87">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B88" t="s">
         <v>150</v>
       </c>
       <c r="C88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>159</v>
       </c>
       <c r="D88" t="s">
         <v>151</v>
       </c>
       <c r="E88">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>160</v>
       </c>
       <c r="F88">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>80</v>
       </c>
       <c r="G88" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('le bébé',1,80);</v>
       </c>
       <c r="H88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the baby',2,80);</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K88" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','80');</v>
+      </c>
+      <c r="M88" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','183');</v>
+      </c>
+      <c r="R88">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B89" t="s">
         <v>152</v>
       </c>
       <c r="C89">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>161</v>
       </c>
       <c r="D89" t="s">
         <v>153</v>
       </c>
       <c r="E89">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>162</v>
       </c>
       <c r="F89">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>81</v>
       </c>
       <c r="G89" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('la femme',1,81);</v>
       </c>
       <c r="H89" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the wife',2,81);</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K89" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','81');</v>
+      </c>
+      <c r="M89" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','184');</v>
+      </c>
+      <c r="R89">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B90" t="s">
         <v>154</v>
       </c>
       <c r="C90">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>163</v>
       </c>
       <c r="D90" t="s">
         <v>155</v>
       </c>
       <c r="E90">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>164</v>
       </c>
       <c r="F90">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>82</v>
       </c>
       <c r="G90" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('la fiancée',1,82);</v>
       </c>
       <c r="H90" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the fiancée',2,82);</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K90" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','82');</v>
+      </c>
+      <c r="M90" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','185');</v>
+      </c>
+      <c r="R90">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B91" t="s">
         <v>156</v>
       </c>
       <c r="C91">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>165</v>
       </c>
       <c r="D91" t="s">
         <v>157</v>
       </c>
       <c r="E91">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>166</v>
       </c>
       <c r="F91">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>83</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('la grand-mère',1,83);</v>
       </c>
       <c r="H91" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the grandmother',2,83);</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K91" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','83');</v>
+      </c>
+      <c r="M91" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','186');</v>
+      </c>
+      <c r="R91">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B92" t="s">
         <v>158</v>
       </c>
       <c r="C92">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>167</v>
       </c>
       <c r="D92" t="s">
         <v>159</v>
       </c>
       <c r="E92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>168</v>
       </c>
       <c r="F92">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>84</v>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('les petits-enfants',1,84);</v>
       </c>
       <c r="H92" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the grandchildren',2,84);</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K92" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','84');</v>
+      </c>
+      <c r="M92" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','187');</v>
+      </c>
+      <c r="R92">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B93" t="s">
         <v>160</v>
       </c>
       <c r="C93">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>169</v>
       </c>
       <c r="D93" t="s">
         <v>161</v>
       </c>
       <c r="E93">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>170</v>
       </c>
       <c r="F93">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>85</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('la tante',1,85);</v>
       </c>
       <c r="H93" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the aunt',2,85);</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K93" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','85');</v>
+      </c>
+      <c r="M93" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','188');</v>
+      </c>
+      <c r="R93">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B94" t="s">
         <v>162</v>
       </c>
       <c r="C94">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>171</v>
       </c>
       <c r="D94" t="s">
         <v>163</v>
       </c>
       <c r="E94">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>172</v>
       </c>
       <c r="F94">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>86</v>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('la nièce',1,86);</v>
       </c>
       <c r="H94" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the niece',2,86);</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K94" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','86');</v>
+      </c>
+      <c r="M94" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','189');</v>
+      </c>
+      <c r="R94">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B95" t="s">
         <v>164</v>
       </c>
       <c r="C95">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>173</v>
       </c>
       <c r="D95" t="s">
         <v>165</v>
       </c>
       <c r="E95">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>174</v>
       </c>
       <c r="F95">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>87</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('la belle-mère',1,87);</v>
       </c>
       <c r="H95" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the step mother',2,87);</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K95" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','87');</v>
+      </c>
+      <c r="M95" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','190');</v>
+      </c>
+      <c r="R95">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B96" t="s">
         <v>166</v>
       </c>
       <c r="C96">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>175</v>
       </c>
       <c r="D96" t="s">
         <v>167</v>
       </c>
       <c r="E96">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>176</v>
       </c>
       <c r="F96">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>88</v>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('la cousine',1,88);</v>
       </c>
       <c r="H96" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the cousin (female)',2,88);</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K96" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','88');</v>
+      </c>
+      <c r="M96" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','191');</v>
+      </c>
+      <c r="R96">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B97" t="s">
         <v>168</v>
       </c>
       <c r="C97">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>177</v>
       </c>
       <c r="D97" t="s">
         <v>169</v>
       </c>
       <c r="E97">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>178</v>
       </c>
       <c r="F97">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>89</v>
       </c>
       <c r="G97" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('la belle-sœur',1,89);</v>
       </c>
       <c r="H97" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('sister in-law',2,89);</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K97" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','89');</v>
+      </c>
+      <c r="M97" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','192');</v>
+      </c>
+      <c r="R97">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B98" t="s">
         <v>170</v>
       </c>
       <c r="C98">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>179</v>
       </c>
       <c r="D98" t="s">
         <v>171</v>
       </c>
       <c r="E98">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>180</v>
       </c>
       <c r="F98">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>90</v>
       </c>
       <c r="G98" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('la mère',1,90);</v>
       </c>
       <c r="H98" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the mother',2,90);</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K98" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','90');</v>
+      </c>
+      <c r="M98" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','193');</v>
+      </c>
+      <c r="R98">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B99" t="s">
         <v>172</v>
       </c>
       <c r="C99">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>181</v>
       </c>
       <c r="D99" t="s">
         <v>196</v>
       </c>
       <c r="E99">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>182</v>
       </c>
       <c r="F99">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>91</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('le frère',1,91);</v>
       </c>
       <c r="H99" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the brother',2,91);</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K99" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','91');</v>
+      </c>
+      <c r="M99" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','194');</v>
+      </c>
+      <c r="R99">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B100" t="s">
         <v>173</v>
       </c>
       <c r="C100">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>183</v>
       </c>
       <c r="D100" t="s">
         <v>174</v>
       </c>
       <c r="E100">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>184</v>
       </c>
       <c r="F100">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>92</v>
       </c>
       <c r="G100" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('le fils',1,92);</v>
       </c>
       <c r="H100" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the son',2,92);</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K100" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','92');</v>
+      </c>
+      <c r="M100" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','195');</v>
+      </c>
+      <c r="R100">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B101" t="s">
         <v>175</v>
       </c>
       <c r="C101">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>185</v>
       </c>
       <c r="D101" t="s">
         <v>176</v>
       </c>
       <c r="E101">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>186</v>
       </c>
       <c r="F101">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>93</v>
       </c>
       <c r="G101" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('l’enfant',1,93);</v>
       </c>
       <c r="H101" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the child',2,93);</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K101" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','93');</v>
+      </c>
+      <c r="M101" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','196');</v>
+      </c>
+      <c r="R101">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B102" t="s">
         <v>177</v>
       </c>
       <c r="C102">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>187</v>
       </c>
       <c r="D102" t="s">
         <v>178</v>
       </c>
       <c r="E102">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>188</v>
       </c>
       <c r="F102">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>94</v>
       </c>
       <c r="G102" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('le mari',1,94);</v>
       </c>
       <c r="H102" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the husband',2,94);</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K102" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','94');</v>
+      </c>
+      <c r="M102" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','197');</v>
+      </c>
+      <c r="R102">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B103" t="s">
         <v>179</v>
       </c>
       <c r="C103">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>189</v>
       </c>
       <c r="D103" t="s">
         <v>180</v>
       </c>
       <c r="E103">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>190</v>
       </c>
       <c r="F103">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>95</v>
       </c>
       <c r="G103" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('le fiancé',1,95);</v>
       </c>
       <c r="H103" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the fiancé',2,95);</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K103" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','95');</v>
+      </c>
+      <c r="M103" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','198');</v>
+      </c>
+      <c r="R103">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B104" t="s">
         <v>181</v>
       </c>
       <c r="C104">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>191</v>
       </c>
       <c r="D104" t="s">
         <v>182</v>
       </c>
       <c r="E104">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>192</v>
       </c>
       <c r="F104">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>96</v>
       </c>
       <c r="G104" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('le grand-père',1,96);</v>
       </c>
       <c r="H104" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the grandfather',2,96);</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K104" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','96');</v>
+      </c>
+      <c r="M104" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','199');</v>
+      </c>
+      <c r="R104">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B105" t="s">
         <v>183</v>
       </c>
       <c r="C105">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>193</v>
       </c>
       <c r="D105" t="s">
         <v>184</v>
       </c>
       <c r="E105">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>194</v>
       </c>
       <c r="F105">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>97</v>
       </c>
       <c r="G105" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('les grand-parents',1,97);</v>
       </c>
       <c r="H105" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the grandparents',2,97);</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K105" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','97');</v>
+      </c>
+      <c r="M105" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','200');</v>
+      </c>
+      <c r="R105">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B106" t="s">
         <v>185</v>
       </c>
       <c r="C106">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>195</v>
       </c>
       <c r="D106" t="s">
         <v>186</v>
       </c>
       <c r="E106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>196</v>
       </c>
       <c r="F106">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>98</v>
       </c>
       <c r="G106" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('l’oncle',1,98);</v>
       </c>
       <c r="H106" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the uncle',2,98);</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K106" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','98');</v>
+      </c>
+      <c r="M106" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','201');</v>
+      </c>
+      <c r="R106">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B107" t="s">
         <v>187</v>
       </c>
       <c r="C107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>197</v>
       </c>
       <c r="D107" t="s">
         <v>188</v>
       </c>
       <c r="E107">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>198</v>
       </c>
       <c r="F107">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>99</v>
       </c>
       <c r="G107" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('le neveu',1,99);</v>
       </c>
       <c r="H107" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the nephew',2,99);</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K107" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','99');</v>
+      </c>
+      <c r="M107" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','202');</v>
+      </c>
+      <c r="R107">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B108" t="s">
         <v>189</v>
       </c>
       <c r="C108">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>199</v>
       </c>
       <c r="D108" t="s">
         <v>190</v>
       </c>
       <c r="E108">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>200</v>
       </c>
       <c r="F108">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>100</v>
       </c>
       <c r="G108" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('le beau-père',1,100);</v>
       </c>
       <c r="H108" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the step father',2,100);</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K108" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','100');</v>
+      </c>
+      <c r="M108" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','203');</v>
+      </c>
+      <c r="R108">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B109" t="s">
         <v>191</v>
       </c>
       <c r="C109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>201</v>
       </c>
       <c r="D109" t="s">
         <v>192</v>
       </c>
       <c r="E109">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>202</v>
       </c>
       <c r="F109">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>101</v>
       </c>
       <c r="G109" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('le cousin',1,101);</v>
       </c>
       <c r="H109" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('the cousin (male)',2,101);</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K109" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','101');</v>
+      </c>
+      <c r="M109" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','204');</v>
+      </c>
+      <c r="R109">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B110" t="s">
         <v>193</v>
       </c>
       <c r="C110">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>203</v>
       </c>
       <c r="D110" t="s">
         <v>194</v>
       </c>
       <c r="E110">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>204</v>
       </c>
       <c r="F110">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>102</v>
       </c>
       <c r="G110" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('le beau-frère',1,102);</v>
       </c>
       <c r="H110" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('brother in-law',2,102);</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K110" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','102');</v>
+      </c>
+      <c r="M110" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','205');</v>
+      </c>
+      <c r="R110">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B111" t="s">
         <v>189</v>
       </c>
       <c r="C111">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>205</v>
       </c>
       <c r="D111" t="s">
         <v>195</v>
       </c>
       <c r="E111">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>206</v>
       </c>
       <c r="F111">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>103</v>
       </c>
       <c r="G111" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('le beau-père',1,103);</v>
       </c>
       <c r="H111" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>INSERT INTO words(value,language_id,semantic_id) VALUES ('father in-law',2,103);</v>
+      </c>
+      <c r="K111" t="str">
+        <f t="shared" si="15"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','103');</v>
+      </c>
+      <c r="M111" t="str">
+        <f t="shared" si="16"/>
+        <v>INSERT INTO contents(theme_id,word_id) VALUES('4','206');</v>
+      </c>
+      <c r="R111">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>